<commit_message>
学习计划更新.10.13 Signed-off-by: lzkmeet599 <511353271@qq.com>
</commit_message>
<xml_diff>
--- a/01每日学习任务.xlsx
+++ b/01每日学习任务.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\0李智凯\00笔记&amp;博客\已备份QQ群笔记\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52CCFFB3-F9C9-4BD3-A2B5-7D994E29F74D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC62D04D-9557-4B58-9940-D8A3DB5B9FF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="29020" windowHeight="17620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>日期</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -47,6 +47,14 @@
   </si>
   <si>
     <t>完成红日红队评估(一)靶场的渗透，并做好笔记</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>实际学习内容</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>没有学习</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -98,7 +106,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -115,6 +123,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -396,10 +407,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D77"/>
+  <dimension ref="A1:E77"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -407,10 +418,11 @@
     <col min="1" max="1" width="15.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="59.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="60.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="60.75" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="5" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="5" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -421,474 +433,561 @@
         <v>4</v>
       </c>
       <c r="D1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>44481</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
+    <row r="3" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
+        <v>44482</v>
+      </c>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
       <c r="D3" s="2"/>
-    </row>
-    <row r="4" spans="1:4" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
-    </row>
-    <row r="5" spans="1:4" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
-    </row>
-    <row r="6" spans="1:4" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
-    </row>
-    <row r="7" spans="1:4" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
-    </row>
-    <row r="8" spans="1:4" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
-    </row>
-    <row r="9" spans="1:4" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
-    </row>
-    <row r="10" spans="1:4" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="E9" s="2"/>
+    </row>
+    <row r="10" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
-    </row>
-    <row r="11" spans="1:4" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="E10" s="2"/>
+    </row>
+    <row r="11" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
-    </row>
-    <row r="12" spans="1:4" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="E11" s="2"/>
+    </row>
+    <row r="12" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
-    </row>
-    <row r="13" spans="1:4" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
-    </row>
-    <row r="14" spans="1:4" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="E13" s="2"/>
+    </row>
+    <row r="14" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
-    </row>
-    <row r="15" spans="1:4" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="E14" s="2"/>
+    </row>
+    <row r="15" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
-    </row>
-    <row r="16" spans="1:4" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="E15" s="2"/>
+    </row>
+    <row r="16" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
-    </row>
-    <row r="17" spans="1:4" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="E16" s="2"/>
+    </row>
+    <row r="17" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
-    </row>
-    <row r="18" spans="1:4" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="E17" s="2"/>
+    </row>
+    <row r="18" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
-    </row>
-    <row r="19" spans="1:4" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="E18" s="2"/>
+    </row>
+    <row r="19" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
-    </row>
-    <row r="20" spans="1:4" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="E19" s="2"/>
+    </row>
+    <row r="20" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
-    </row>
-    <row r="21" spans="1:4" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="E20" s="2"/>
+    </row>
+    <row r="21" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
-    </row>
-    <row r="22" spans="1:4" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="E21" s="2"/>
+    </row>
+    <row r="22" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
-    </row>
-    <row r="23" spans="1:4" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="E22" s="2"/>
+    </row>
+    <row r="23" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
-    </row>
-    <row r="24" spans="1:4" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="E23" s="2"/>
+    </row>
+    <row r="24" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
-    </row>
-    <row r="25" spans="1:4" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="E24" s="2"/>
+    </row>
+    <row r="25" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
-    </row>
-    <row r="26" spans="1:4" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="E25" s="2"/>
+    </row>
+    <row r="26" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
-    </row>
-    <row r="27" spans="1:4" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="E26" s="2"/>
+    </row>
+    <row r="27" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
-    </row>
-    <row r="28" spans="1:4" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="E27" s="2"/>
+    </row>
+    <row r="28" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
-    </row>
-    <row r="29" spans="1:4" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="E28" s="2"/>
+    </row>
+    <row r="29" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
-    </row>
-    <row r="30" spans="1:4" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="E29" s="2"/>
+    </row>
+    <row r="30" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
-    </row>
-    <row r="31" spans="1:4" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="E30" s="2"/>
+    </row>
+    <row r="31" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
-    </row>
-    <row r="32" spans="1:4" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="E31" s="2"/>
+    </row>
+    <row r="32" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
-    </row>
-    <row r="33" spans="1:4" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="E32" s="2"/>
+    </row>
+    <row r="33" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
-    </row>
-    <row r="34" spans="1:4" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="E33" s="2"/>
+    </row>
+    <row r="34" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
-    </row>
-    <row r="35" spans="1:4" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="E34" s="2"/>
+    </row>
+    <row r="35" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
-    </row>
-    <row r="36" spans="1:4" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="E35" s="2"/>
+    </row>
+    <row r="36" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
-    </row>
-    <row r="37" spans="1:4" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="E36" s="2"/>
+    </row>
+    <row r="37" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
-    </row>
-    <row r="38" spans="1:4" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="E37" s="2"/>
+    </row>
+    <row r="38" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
-    </row>
-    <row r="39" spans="1:4" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="E38" s="2"/>
+    </row>
+    <row r="39" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
-    </row>
-    <row r="40" spans="1:4" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="E39" s="2"/>
+    </row>
+    <row r="40" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
-    </row>
-    <row r="41" spans="1:4" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="E40" s="2"/>
+    </row>
+    <row r="41" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
-    </row>
-    <row r="42" spans="1:4" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="E41" s="2"/>
+    </row>
+    <row r="42" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
-    </row>
-    <row r="43" spans="1:4" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="E42" s="2"/>
+    </row>
+    <row r="43" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
-    </row>
-    <row r="44" spans="1:4" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="E43" s="2"/>
+    </row>
+    <row r="44" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
-    </row>
-    <row r="45" spans="1:4" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="E44" s="2"/>
+    </row>
+    <row r="45" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
-    </row>
-    <row r="46" spans="1:4" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="E45" s="2"/>
+    </row>
+    <row r="46" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
-    </row>
-    <row r="47" spans="1:4" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="E46" s="2"/>
+    </row>
+    <row r="47" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
-    </row>
-    <row r="48" spans="1:4" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="E47" s="2"/>
+    </row>
+    <row r="48" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
-    </row>
-    <row r="49" spans="1:4" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="E48" s="2"/>
+    </row>
+    <row r="49" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
-    </row>
-    <row r="50" spans="1:4" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="E49" s="2"/>
+    </row>
+    <row r="50" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A50" s="2"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
       <c r="D50" s="2"/>
-    </row>
-    <row r="51" spans="1:4" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="E50" s="2"/>
+    </row>
+    <row r="51" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A51" s="2"/>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
-    </row>
-    <row r="52" spans="1:4" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="E51" s="2"/>
+    </row>
+    <row r="52" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A52" s="2"/>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
-    </row>
-    <row r="53" spans="1:4" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="E52" s="2"/>
+    </row>
+    <row r="53" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A53" s="2"/>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
-    </row>
-    <row r="54" spans="1:4" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="E53" s="2"/>
+    </row>
+    <row r="54" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A54" s="2"/>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
-    </row>
-    <row r="55" spans="1:4" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="E54" s="2"/>
+    </row>
+    <row r="55" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A55" s="2"/>
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
-    </row>
-    <row r="56" spans="1:4" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="E55" s="2"/>
+    </row>
+    <row r="56" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A56" s="2"/>
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
       <c r="D56" s="2"/>
-    </row>
-    <row r="57" spans="1:4" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="E56" s="2"/>
+    </row>
+    <row r="57" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A57" s="2"/>
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
-    </row>
-    <row r="58" spans="1:4" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="E57" s="2"/>
+    </row>
+    <row r="58" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A58" s="2"/>
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
-    </row>
-    <row r="59" spans="1:4" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="E58" s="2"/>
+    </row>
+    <row r="59" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A59" s="2"/>
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
       <c r="D59" s="2"/>
-    </row>
-    <row r="60" spans="1:4" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="E59" s="2"/>
+    </row>
+    <row r="60" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A60" s="2"/>
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
       <c r="D60" s="2"/>
-    </row>
-    <row r="61" spans="1:4" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="E60" s="2"/>
+    </row>
+    <row r="61" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A61" s="2"/>
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
       <c r="D61" s="2"/>
-    </row>
-    <row r="62" spans="1:4" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="E61" s="2"/>
+    </row>
+    <row r="62" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A62" s="2"/>
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
-    </row>
-    <row r="63" spans="1:4" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="E62" s="2"/>
+    </row>
+    <row r="63" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A63" s="2"/>
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
       <c r="D63" s="2"/>
-    </row>
-    <row r="64" spans="1:4" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="E63" s="2"/>
+    </row>
+    <row r="64" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A64" s="2"/>
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
       <c r="D64" s="2"/>
-    </row>
-    <row r="65" spans="1:4" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="E64" s="2"/>
+    </row>
+    <row r="65" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A65" s="2"/>
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
       <c r="D65" s="2"/>
-    </row>
-    <row r="66" spans="1:4" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="E65" s="2"/>
+    </row>
+    <row r="66" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A66" s="2"/>
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
       <c r="D66" s="2"/>
-    </row>
-    <row r="67" spans="1:4" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="E66" s="2"/>
+    </row>
+    <row r="67" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A67" s="2"/>
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
       <c r="D67" s="2"/>
-    </row>
-    <row r="68" spans="1:4" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="E67" s="2"/>
+    </row>
+    <row r="68" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A68" s="2"/>
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
       <c r="D68" s="2"/>
-    </row>
-    <row r="69" spans="1:4" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="E68" s="2"/>
+    </row>
+    <row r="69" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A69" s="2"/>
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
       <c r="D69" s="2"/>
-    </row>
-    <row r="70" spans="1:4" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="E69" s="2"/>
+    </row>
+    <row r="70" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A70" s="2"/>
       <c r="B70" s="2"/>
       <c r="C70" s="2"/>
       <c r="D70" s="2"/>
-    </row>
-    <row r="71" spans="1:4" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="E70" s="2"/>
+    </row>
+    <row r="71" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A71" s="2"/>
       <c r="B71" s="2"/>
       <c r="C71" s="2"/>
       <c r="D71" s="2"/>
-    </row>
-    <row r="72" spans="1:4" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="E71" s="2"/>
+    </row>
+    <row r="72" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A72" s="2"/>
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
       <c r="D72" s="2"/>
-    </row>
-    <row r="73" spans="1:4" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="E72" s="2"/>
+    </row>
+    <row r="73" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A73" s="2"/>
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
       <c r="D73" s="2"/>
-    </row>
-    <row r="74" spans="1:4" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="E73" s="2"/>
+    </row>
+    <row r="74" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A74" s="2"/>
       <c r="B74" s="2"/>
       <c r="C74" s="2"/>
       <c r="D74" s="2"/>
-    </row>
-    <row r="75" spans="1:4" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="E74" s="2"/>
+    </row>
+    <row r="75" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A75" s="2"/>
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
       <c r="D75" s="2"/>
-    </row>
-    <row r="76" spans="1:4" ht="20" x14ac:dyDescent="0.4">
+      <c r="E75" s="2"/>
+    </row>
+    <row r="76" spans="1:5" ht="20" x14ac:dyDescent="0.4">
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
       <c r="D76" s="1"/>
-    </row>
-    <row r="77" spans="1:4" ht="20" x14ac:dyDescent="0.4">
+      <c r="E76" s="1"/>
+    </row>
+    <row r="77" spans="1:5" ht="20" x14ac:dyDescent="0.4">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
       <c r="D77" s="1"/>
+      <c r="E77" s="1"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
靶场介绍、外围打点完成2021-10-13 Signed-off-by: lzkmeet599 <511353271@qq.com>
</commit_message>
<xml_diff>
--- a/01每日学习任务.xlsx
+++ b/01每日学习任务.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\0李智凯\00笔记&amp;博客\已备份QQ群笔记\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC62D04D-9557-4B58-9940-D8A3DB5B9FF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A895319E-F03F-4503-867C-EA2C4E79B6A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="29020" windowHeight="17620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>日期</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -55,6 +55,37 @@
   </si>
   <si>
     <t>没有学习</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>后续学习任务</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1 获取服务器权限后添加用户的几种方法</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">2 关闭防火墙、查看防火墙状态的方法 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>笔记文档名</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>红日靶场(一)渗透</t>
+  </si>
+  <si>
+    <t>是否备份qq群</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>否</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>完成外围打点获取win7服务器shell</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -86,12 +117,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -106,7 +143,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -126,6 +163,15 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -407,586 +453,767 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E77"/>
+  <dimension ref="A1:G78"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.08203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="59.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="60.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="60.75" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="60.75" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="5" customFormat="1" ht="20" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:7" s="8" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="5" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E2" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
-      <c r="A2" s="3">
+    <row r="3" spans="1:7" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
         <v>44481</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="10">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
-      <c r="A3" s="3">
+    <row r="4" spans="1:7" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
         <v>44482</v>
       </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-    </row>
-    <row r="4" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-    </row>
-    <row r="5" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="10">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
-    </row>
-    <row r="6" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:7" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
-    </row>
-    <row r="7" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:7" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
-    </row>
-    <row r="8" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="1:7" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
-    </row>
-    <row r="9" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="1:7" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
-    </row>
-    <row r="10" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+    </row>
+    <row r="10" spans="1:7" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
-    </row>
-    <row r="11" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+    </row>
+    <row r="11" spans="1:7" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
-    </row>
-    <row r="12" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+    </row>
+    <row r="12" spans="1:7" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
-    </row>
-    <row r="13" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+    </row>
+    <row r="13" spans="1:7" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
-    </row>
-    <row r="14" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+    </row>
+    <row r="14" spans="1:7" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
-    </row>
-    <row r="15" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+    </row>
+    <row r="15" spans="1:7" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
-    </row>
-    <row r="16" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+    </row>
+    <row r="16" spans="1:7" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
-    </row>
-    <row r="17" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+    </row>
+    <row r="17" spans="1:7" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
-    </row>
-    <row r="18" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+    </row>
+    <row r="18" spans="1:7" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
-    </row>
-    <row r="19" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+    </row>
+    <row r="19" spans="1:7" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
-    </row>
-    <row r="20" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+    </row>
+    <row r="20" spans="1:7" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
-    </row>
-    <row r="21" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+    </row>
+    <row r="21" spans="1:7" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
-    </row>
-    <row r="22" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+    </row>
+    <row r="22" spans="1:7" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
-    </row>
-    <row r="23" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+    </row>
+    <row r="23" spans="1:7" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
-    </row>
-    <row r="24" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+    </row>
+    <row r="24" spans="1:7" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
-    </row>
-    <row r="25" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+    </row>
+    <row r="25" spans="1:7" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
-    </row>
-    <row r="26" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+    </row>
+    <row r="26" spans="1:7" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
-    </row>
-    <row r="27" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+    </row>
+    <row r="27" spans="1:7" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
-    </row>
-    <row r="28" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+    </row>
+    <row r="28" spans="1:7" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
-    </row>
-    <row r="29" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+    </row>
+    <row r="29" spans="1:7" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
-    </row>
-    <row r="30" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+    </row>
+    <row r="30" spans="1:7" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
-    </row>
-    <row r="31" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+    </row>
+    <row r="31" spans="1:7" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
-    </row>
-    <row r="32" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+    </row>
+    <row r="32" spans="1:7" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
-    </row>
-    <row r="33" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+    </row>
+    <row r="33" spans="1:7" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
-    </row>
-    <row r="34" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+    </row>
+    <row r="34" spans="1:7" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
-    </row>
-    <row r="35" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+    </row>
+    <row r="35" spans="1:7" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
-    </row>
-    <row r="36" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+    </row>
+    <row r="36" spans="1:7" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
-    </row>
-    <row r="37" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+    </row>
+    <row r="37" spans="1:7" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
-    </row>
-    <row r="38" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+    </row>
+    <row r="38" spans="1:7" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
-    </row>
-    <row r="39" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+    </row>
+    <row r="39" spans="1:7" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
-    </row>
-    <row r="40" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
+    </row>
+    <row r="40" spans="1:7" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
-    </row>
-    <row r="41" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="F40" s="2"/>
+      <c r="G40" s="2"/>
+    </row>
+    <row r="41" spans="1:7" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
-    </row>
-    <row r="42" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="F41" s="2"/>
+      <c r="G41" s="2"/>
+    </row>
+    <row r="42" spans="1:7" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
-    </row>
-    <row r="43" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="F42" s="2"/>
+      <c r="G42" s="2"/>
+    </row>
+    <row r="43" spans="1:7" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
       <c r="E43" s="2"/>
-    </row>
-    <row r="44" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="F43" s="2"/>
+      <c r="G43" s="2"/>
+    </row>
+    <row r="44" spans="1:7" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
       <c r="E44" s="2"/>
-    </row>
-    <row r="45" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="F44" s="2"/>
+      <c r="G44" s="2"/>
+    </row>
+    <row r="45" spans="1:7" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
-    </row>
-    <row r="46" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="F45" s="2"/>
+      <c r="G45" s="2"/>
+    </row>
+    <row r="46" spans="1:7" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
-    </row>
-    <row r="47" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="F46" s="2"/>
+      <c r="G46" s="2"/>
+    </row>
+    <row r="47" spans="1:7" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
       <c r="E47" s="2"/>
-    </row>
-    <row r="48" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="F47" s="2"/>
+      <c r="G47" s="2"/>
+    </row>
+    <row r="48" spans="1:7" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
       <c r="E48" s="2"/>
-    </row>
-    <row r="49" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="F48" s="2"/>
+      <c r="G48" s="2"/>
+    </row>
+    <row r="49" spans="1:7" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
       <c r="E49" s="2"/>
-    </row>
-    <row r="50" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="F49" s="2"/>
+      <c r="G49" s="2"/>
+    </row>
+    <row r="50" spans="1:7" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A50" s="2"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
       <c r="D50" s="2"/>
       <c r="E50" s="2"/>
-    </row>
-    <row r="51" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="F50" s="2"/>
+      <c r="G50" s="2"/>
+    </row>
+    <row r="51" spans="1:7" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A51" s="2"/>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
       <c r="E51" s="2"/>
-    </row>
-    <row r="52" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="F51" s="2"/>
+      <c r="G51" s="2"/>
+    </row>
+    <row r="52" spans="1:7" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A52" s="2"/>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
       <c r="E52" s="2"/>
-    </row>
-    <row r="53" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="F52" s="2"/>
+      <c r="G52" s="2"/>
+    </row>
+    <row r="53" spans="1:7" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A53" s="2"/>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
       <c r="E53" s="2"/>
-    </row>
-    <row r="54" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="F53" s="2"/>
+      <c r="G53" s="2"/>
+    </row>
+    <row r="54" spans="1:7" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A54" s="2"/>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
       <c r="E54" s="2"/>
-    </row>
-    <row r="55" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="F54" s="2"/>
+      <c r="G54" s="2"/>
+    </row>
+    <row r="55" spans="1:7" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A55" s="2"/>
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
       <c r="E55" s="2"/>
-    </row>
-    <row r="56" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="F55" s="2"/>
+      <c r="G55" s="2"/>
+    </row>
+    <row r="56" spans="1:7" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A56" s="2"/>
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
       <c r="D56" s="2"/>
       <c r="E56" s="2"/>
-    </row>
-    <row r="57" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="F56" s="2"/>
+      <c r="G56" s="2"/>
+    </row>
+    <row r="57" spans="1:7" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A57" s="2"/>
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
       <c r="E57" s="2"/>
-    </row>
-    <row r="58" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="F57" s="2"/>
+      <c r="G57" s="2"/>
+    </row>
+    <row r="58" spans="1:7" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A58" s="2"/>
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
       <c r="E58" s="2"/>
-    </row>
-    <row r="59" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="F58" s="2"/>
+      <c r="G58" s="2"/>
+    </row>
+    <row r="59" spans="1:7" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A59" s="2"/>
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
       <c r="D59" s="2"/>
       <c r="E59" s="2"/>
-    </row>
-    <row r="60" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="F59" s="2"/>
+      <c r="G59" s="2"/>
+    </row>
+    <row r="60" spans="1:7" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A60" s="2"/>
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
       <c r="D60" s="2"/>
       <c r="E60" s="2"/>
-    </row>
-    <row r="61" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="F60" s="2"/>
+      <c r="G60" s="2"/>
+    </row>
+    <row r="61" spans="1:7" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A61" s="2"/>
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
       <c r="D61" s="2"/>
       <c r="E61" s="2"/>
-    </row>
-    <row r="62" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="F61" s="2"/>
+      <c r="G61" s="2"/>
+    </row>
+    <row r="62" spans="1:7" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A62" s="2"/>
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
       <c r="E62" s="2"/>
-    </row>
-    <row r="63" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="F62" s="2"/>
+      <c r="G62" s="2"/>
+    </row>
+    <row r="63" spans="1:7" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A63" s="2"/>
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
       <c r="D63" s="2"/>
       <c r="E63" s="2"/>
-    </row>
-    <row r="64" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="F63" s="2"/>
+      <c r="G63" s="2"/>
+    </row>
+    <row r="64" spans="1:7" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A64" s="2"/>
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
       <c r="D64" s="2"/>
       <c r="E64" s="2"/>
-    </row>
-    <row r="65" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="F64" s="2"/>
+      <c r="G64" s="2"/>
+    </row>
+    <row r="65" spans="1:7" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A65" s="2"/>
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
       <c r="D65" s="2"/>
       <c r="E65" s="2"/>
-    </row>
-    <row r="66" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="F65" s="2"/>
+      <c r="G65" s="2"/>
+    </row>
+    <row r="66" spans="1:7" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A66" s="2"/>
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
       <c r="D66" s="2"/>
       <c r="E66" s="2"/>
-    </row>
-    <row r="67" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="F66" s="2"/>
+      <c r="G66" s="2"/>
+    </row>
+    <row r="67" spans="1:7" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A67" s="2"/>
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
       <c r="D67" s="2"/>
       <c r="E67" s="2"/>
-    </row>
-    <row r="68" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="F67" s="2"/>
+      <c r="G67" s="2"/>
+    </row>
+    <row r="68" spans="1:7" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A68" s="2"/>
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
       <c r="D68" s="2"/>
       <c r="E68" s="2"/>
-    </row>
-    <row r="69" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="F68" s="2"/>
+      <c r="G68" s="2"/>
+    </row>
+    <row r="69" spans="1:7" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A69" s="2"/>
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
       <c r="D69" s="2"/>
       <c r="E69" s="2"/>
-    </row>
-    <row r="70" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="F69" s="2"/>
+      <c r="G69" s="2"/>
+    </row>
+    <row r="70" spans="1:7" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A70" s="2"/>
       <c r="B70" s="2"/>
       <c r="C70" s="2"/>
       <c r="D70" s="2"/>
       <c r="E70" s="2"/>
-    </row>
-    <row r="71" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="F70" s="2"/>
+      <c r="G70" s="2"/>
+    </row>
+    <row r="71" spans="1:7" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A71" s="2"/>
       <c r="B71" s="2"/>
       <c r="C71" s="2"/>
       <c r="D71" s="2"/>
       <c r="E71" s="2"/>
-    </row>
-    <row r="72" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="F71" s="2"/>
+      <c r="G71" s="2"/>
+    </row>
+    <row r="72" spans="1:7" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A72" s="2"/>
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
       <c r="D72" s="2"/>
       <c r="E72" s="2"/>
-    </row>
-    <row r="73" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="F72" s="2"/>
+      <c r="G72" s="2"/>
+    </row>
+    <row r="73" spans="1:7" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A73" s="2"/>
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
       <c r="D73" s="2"/>
       <c r="E73" s="2"/>
-    </row>
-    <row r="74" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="F73" s="2"/>
+      <c r="G73" s="2"/>
+    </row>
+    <row r="74" spans="1:7" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A74" s="2"/>
       <c r="B74" s="2"/>
       <c r="C74" s="2"/>
       <c r="D74" s="2"/>
       <c r="E74" s="2"/>
-    </row>
-    <row r="75" spans="1:5" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="F74" s="2"/>
+      <c r="G74" s="2"/>
+    </row>
+    <row r="75" spans="1:7" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A75" s="2"/>
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
       <c r="D75" s="2"/>
       <c r="E75" s="2"/>
-    </row>
-    <row r="76" spans="1:5" ht="20" x14ac:dyDescent="0.4">
-      <c r="A76" s="1"/>
-      <c r="B76" s="1"/>
-      <c r="C76" s="1"/>
-      <c r="D76" s="1"/>
-      <c r="E76" s="1"/>
-    </row>
-    <row r="77" spans="1:5" ht="20" x14ac:dyDescent="0.4">
+      <c r="F75" s="2"/>
+      <c r="G75" s="2"/>
+    </row>
+    <row r="76" spans="1:7" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
+      <c r="A76" s="2"/>
+      <c r="B76" s="2"/>
+      <c r="C76" s="2"/>
+      <c r="D76" s="2"/>
+      <c r="E76" s="2"/>
+      <c r="F76" s="2"/>
+      <c r="G76" s="2"/>
+    </row>
+    <row r="77" spans="1:7" ht="20" x14ac:dyDescent="0.4">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
       <c r="D77" s="1"/>
       <c r="E77" s="1"/>
+      <c r="F77" s="1"/>
+      <c r="G77" s="1"/>
+    </row>
+    <row r="78" spans="1:7" ht="20" x14ac:dyDescent="0.4">
+      <c r="A78" s="1"/>
+      <c r="B78" s="1"/>
+      <c r="C78" s="1"/>
+      <c r="D78" s="1"/>
+      <c r="E78" s="1"/>
+      <c r="F78" s="1"/>
+      <c r="G78" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
更新学习任务 最近杂事多没有学习...2021-10-17 Signed-off-by: lzkmeet599 <511353271@qq.com>
</commit_message>
<xml_diff>
--- a/01每日学习任务.xlsx
+++ b/01每日学习任务.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\0李智凯\00笔记&amp;博客\已备份QQ群笔记\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA2F6DCA-3440-4856-BE06-305508AD9787}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BE5A387-4EAC-49D5-8E4A-A937E0E6CC34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="29020" windowHeight="17620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
   <si>
     <t>日期</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -38,9 +38,6 @@
   <si>
     <t>完成情况</t>
     <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>http://vulnstack.qiyuanxuetang.net/vuln/detail/2/</t>
   </si>
   <si>
     <t>资源以及文献参考</t>
@@ -104,6 +101,14 @@
   </si>
   <si>
     <t>windows常用命令</t>
+  </si>
+  <si>
+    <t>http://vulnstack.qiyuanxuetang.net/vuln/detail/2/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>无</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -478,8 +483,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -493,13 +498,13 @@
   <sheetData>
     <row r="1" spans="1:7" s="8" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="C1" s="8" t="s">
         <v>9</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="5" customFormat="1" ht="20" x14ac:dyDescent="0.3">
@@ -510,16 +515,16 @@
         <v>1</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>2</v>
@@ -530,19 +535,19 @@
         <v>44481</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G3" s="10">
         <v>0</v>
@@ -555,53 +560,77 @@
       <c r="B4" s="12"/>
       <c r="C4" s="12"/>
       <c r="D4" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="F4" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G4" s="10">
         <v>0.15</v>
       </c>
     </row>
     <row r="5" spans="1:7" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
+      <c r="A5" s="3">
+        <v>44483</v>
+      </c>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
+      <c r="G5" s="10">
+        <v>0.15</v>
+      </c>
     </row>
     <row r="6" spans="1:7" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
+      <c r="A6" s="3">
+        <v>44484</v>
+      </c>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
+      <c r="G6" s="10">
+        <v>0.15</v>
+      </c>
     </row>
     <row r="7" spans="1:7" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
+      <c r="A7" s="3">
+        <v>44485</v>
+      </c>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
+      <c r="G7" s="10">
+        <v>0.15</v>
+      </c>
     </row>
     <row r="8" spans="1:7" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
+      <c r="A8" s="3">
+        <v>44486</v>
+      </c>
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
+      <c r="G8" s="10">
+        <v>0.15</v>
+      </c>
     </row>
     <row r="9" spans="1:7" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
@@ -1235,8 +1264,8 @@
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="B3:B8"/>
+    <mergeCell ref="C3:C8"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1261,13 +1290,13 @@
   <sheetData>
     <row r="1" spans="1:37" ht="20" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D1" s="9"/>
       <c r="E1" s="9"/>
@@ -1306,13 +1335,13 @@
     </row>
     <row r="2" spans="1:37" ht="20" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
@@ -1351,13 +1380,13 @@
     </row>
     <row r="3" spans="1:37" ht="20" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>

</xml_diff>